<commit_message>
add org graph plot
</commit_message>
<xml_diff>
--- a/ReadMe.xlsx
+++ b/ReadMe.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\my_program\kyo-pro\80_AutoPlot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E468EE9-6E90-4567-ABBB-AA3EC0516A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720880FD-A15E-4D6F-86BF-D730F3AC7B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-660" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="備忘録" sheetId="3" r:id="rId2"/>
+    <sheet name="デザイン" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>フォルダ構成</t>
     <rPh sb="4" eb="6">
@@ -162,6 +164,29 @@
   </si>
   <si>
     <t>MainViewModel 表示用に参照</t>
+  </si>
+  <si>
+    <t>見た目はここまで</t>
+    <rPh sb="0" eb="1">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>メ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>グラフの数値自体は読めてるっぽい</t>
+    <rPh sb="4" eb="6">
+      <t>スウチ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジタイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -232,12 +257,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -253,6 +279,432 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1112337</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>277989</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>58198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBC07FA3-DDE5-7B42-A4C6-E1BDCEE7CB53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1772737" y="558800"/>
+          <a:ext cx="4931452" cy="2928398"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C6F813-83FD-14B1-E3CE-8EB464F5EFDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1809750" y="1073150"/>
+          <a:ext cx="4851400" cy="2921000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14181FC3-FB4B-46AD-BD86-78AEE0D248CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1962150" y="1225550"/>
+          <a:ext cx="1803400" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>画像パス入力エリア</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8D224F8-D6B8-49BD-81E0-F3E24CFC1C23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1974850" y="1758950"/>
+          <a:ext cx="2057400" cy="1949450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>入力された画像を表示</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFEA4240-4C51-442D-9C3D-022003EEA05C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="1771650"/>
+          <a:ext cx="2057400" cy="1949450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>読み取った数値をグラフ化した画像を表示</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9249EC5B-CB9B-44F1-ADB5-43E8A024F496}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4083050" y="1225550"/>
+          <a:ext cx="1181100" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>パス決定ボタン</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,13 +972,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView showGridLines="0" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.45"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -1188,4 +1640,55 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D72983-064B-463F-9A5B-81F9920F7E92}">
+  <dimension ref="B2:C18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="5">
+        <v>46018</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F838AA-6B65-4D16-B1B0-EFB7DFB1F921}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>